<commit_message>
Python 3, Header validator, new examples
</commit_message>
<xml_diff>
--- a/example/excel.xlsx
+++ b/example/excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\excel_validator\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\a.elesin\excel_validator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52282D59-533D-48CF-A4B0-1574D938D060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6474"/>
+    <workbookView xWindow="28680" yWindow="1875" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -41,12 +42,6 @@
     <t>Order Date</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -108,13 +103,25 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>неверно</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>First 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +148,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -151,12 +167,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,21 +179,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Вывод" xfId="2" builtinId="21"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -194,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -234,7 +269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -340,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -489,173 +524,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.578125" customWidth="1"/>
-    <col min="3" max="3" width="12.734375" customWidth="1"/>
-    <col min="7" max="7" width="16.9453125" customWidth="1"/>
-    <col min="10" max="10" width="12.3125" customWidth="1"/>
-    <col min="11" max="11" width="12.62890625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2">
-        <v>11</v>
-      </c>
-      <c r="K2" s="1">
-        <v>30472</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1">
+        <v>30472</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="J3">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4">
         <v>9</v>
       </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" t="s">
-        <v>17</v>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6">
         <v>101</v>
       </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>